<commit_message>
Actualicé el archivo, agregando 2 cambios adicionales.
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Cambios/Solicitud_Cambios_160627.xlsx
+++ b/Proyectos/2016/Cambios/Solicitud_Cambios_160627.xlsx
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>Datos Generales</t>
   </si>
@@ -248,9 +248,6 @@
     <t>Ricardo Novela</t>
   </si>
   <si>
-    <t>Adicionar 2 productos al Catálogo de productos relacionados con la creación de una Página Web.</t>
-  </si>
-  <si>
     <t>Se requiere para una página web</t>
   </si>
   <si>
@@ -260,12 +257,6 @@
     <t>AJ</t>
   </si>
   <si>
-    <t>Cambio 1: Adquisición de Domino para página web</t>
-  </si>
-  <si>
-    <t>Cambio 2: Adquisición de hosting para página web</t>
-  </si>
-  <si>
     <t>Para ambos cambios se debe seguir los siguientes procesos</t>
   </si>
   <si>
@@ -285,6 +276,25 @@
   </si>
   <si>
     <t>Notificar en Chat Bitrix de la adición de los 2 productos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adicionar 4 productos al Catálogo de productos </t>
+  </si>
+  <si>
+    <t>Cambio 3: Servicio de Atención a Clientes.
+Precio: $2,950+IVA</t>
+  </si>
+  <si>
+    <t>Cambio 4: Servicio Integral de Ventas
+Precio: $4550+IVA</t>
+  </si>
+  <si>
+    <t>Cambio 2: Adquisición de hosting para página web
+Precio: $2,145+IVA</t>
+  </si>
+  <si>
+    <t>Cambio 1: Adquisición de Domino para página web
+Precio: $644.97+IVA</t>
   </si>
 </sst>
 </file>
@@ -866,7 +876,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="45" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -924,12 +934,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="26" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -944,6 +948,15 @@
     </xf>
     <xf numFmtId="14" fontId="22" fillId="0" borderId="11" xfId="45" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1588,8 +1601,8 @@
   </sheetPr>
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1869,12 +1882,12 @@
     </row>
     <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="17"/>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
@@ -1884,14 +1897,14 @@
       <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="28" t="s">
+      <c r="C3" s="28"/>
+      <c r="D3" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="28"/>
+      <c r="E3" s="26"/>
       <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1902,14 +1915,14 @@
       <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="28" t="s">
+      <c r="C4" s="28"/>
+      <c r="D4" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1920,12 +1933,12 @@
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1935,72 +1948,72 @@
       <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="28" t="s">
+      <c r="C6" s="28"/>
+      <c r="D6" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="28"/>
+      <c r="E6" s="26"/>
       <c r="G6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="29">
+      <c r="C7" s="28"/>
+      <c r="D7" s="27">
         <v>42548</v>
       </c>
-      <c r="E7" s="29"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="28" t="s">
+      <c r="C8" s="28"/>
+      <c r="D8" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="26"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="28"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="28" t="s">
+      <c r="E9" s="26"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="28"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="28"/>
+      <c r="E10" s="26"/>
     </row>
     <row r="11" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
     </row>
     <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B12" s="20" t="s">
@@ -2027,10 +2040,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19"/>
       <c r="C13" s="7" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
@@ -2040,10 +2053,10 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:10" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19"/>
       <c r="C14" s="21" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="8"/>
@@ -2053,10 +2066,10 @@
       <c r="I14" s="7"/>
       <c r="J14" s="21"/>
     </row>
-    <row r="15" spans="1:10" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19"/>
       <c r="C15" s="7" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
@@ -2067,136 +2080,140 @@
       <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="19" t="s">
-        <v>44</v>
-      </c>
+      <c r="B16" s="19"/>
       <c r="C16" s="7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="8">
-        <v>42548</v>
-      </c>
+      <c r="E16" s="8"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="J16" s="21">
-        <f t="shared" ref="J16:J20" si="0">+I16*32.15</f>
-        <v>3.2149999999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>49</v>
+      <c r="I16" s="7"/>
+      <c r="J16" s="21"/>
+    </row>
+    <row r="17" spans="1:10" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="19"/>
+      <c r="C17" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="D17" s="7"/>
-      <c r="E17" s="8">
-        <v>42548</v>
-      </c>
+      <c r="E17" s="8"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-      <c r="I17" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="J17" s="21">
-        <f t="shared" si="0"/>
-        <v>6.43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="51" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="I17" s="7"/>
+      <c r="J17" s="21"/>
+    </row>
+    <row r="18" spans="1:10" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="22"/>
       <c r="E18" s="8">
         <v>42548</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7">
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22">
         <v>0.1</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="22">
+        <f t="shared" ref="J18:J22" si="0">+I18*32.15</f>
+        <v>3.2149999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="8">
+        <v>42548</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="J19" s="22">
+        <f t="shared" si="0"/>
+        <v>9.6449999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="51" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="8">
+        <v>42548</v>
+      </c>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="J20" s="22">
         <f t="shared" si="0"/>
         <v>3.2149999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8">
+    <row r="21" spans="1:10" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="8">
         <v>42548</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7">
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22">
         <v>0.1</v>
       </c>
-      <c r="J19" s="21">
+      <c r="J21" s="22">
         <f t="shared" si="0"/>
         <v>3.2149999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8">
+    <row r="22" spans="1:10" ht="25.5" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="22"/>
+      <c r="E22" s="8">
         <v>42549</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7">
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22">
         <v>0.1</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J22" s="22">
         <f t="shared" si="0"/>
         <v>3.2149999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="19"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="19"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
     </row>
     <row r="23" spans="1:10" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B23" s="19"/>
@@ -2215,7 +2232,7 @@
       </c>
       <c r="D24" s="10">
         <f>SUM(I13:I23)</f>
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2225,10 +2242,10 @@
     <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="24"/>
+      <c r="D26" s="30"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
@@ -2238,7 +2255,7 @@
       </c>
       <c r="D27" s="18">
         <f>SUM(J13:J23)</f>
-        <v>19.29</v>
+        <v>22.504999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -2284,10 +2301,10 @@
     <row r="33" spans="1:4" ht="18.75" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="23"/>
+      <c r="D33" s="29"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="12"/>
@@ -2313,6 +2330,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C26:D26"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B11:J11"/>
@@ -2329,9 +2349,6 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C26:D26"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D29">
@@ -2355,6 +2372,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="$Resources:CType_PWS_Document(1)" ma:contentTypeID="0x0101008A98423170284BEEB635F43C3CF4E98B001A4A1163653B6846ADC5D60A25EBD429" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="e2271a139a2b8ee801614f6b11c48dd3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="035E5738-9077-49AA-867C-265905AEBD06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7346a5ed0265b509ea77989a5de5de18" ns2:_="">
     <xsd:import namespace="035E5738-9077-49AA-867C-265905AEBD06"/>
@@ -2438,15 +2464,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -2463,6 +2480,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F292331-53F9-4EF7-AEE3-BD24EFCEB3B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9B730C3-1047-4794-B798-57186B6BC346}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2475,14 +2500,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F292331-53F9-4EF7-AEE3-BD24EFCEB3B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>